<commit_message>
added Test Cases documentation for Asssignment A
</commit_message>
<xml_diff>
--- a/Documentation/Tests Documents.xlsx
+++ b/Documentation/Tests Documents.xlsx
@@ -1,26 +1,147 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gquispe\Documents\Stensul\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B10528-3315-446C-9779-698B821D68F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DF972AE6-939A-434D-A067-644AAF37E1F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
+    <t>Test Case Procedure</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Navigate to http://immense-hollows-74271.herokuapp.com/
+2:  
+3: 
+4: 
+</t>
+  </si>
+  <si>
+    <t>Create an item</t>
+  </si>
+  <si>
+    <t>Edit another existing item</t>
+  </si>
+  <si>
+    <t>Delete the item created</t>
+  </si>
+  <si>
+    <t>Check max long in description</t>
+  </si>
+  <si>
+    <t>5- Check if exist in the list the item with text “ Creators: Matt Duffer, Ross Duffer ”</t>
+  </si>
+  <si>
+    <t>The new item should be displayed on the "List of Items" section.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1: Navigate to http://immense-hollows-74271.herokuapp.com/
+2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Click the button "Choose a file" and select a jpg image</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3: Enter the item description on the "Item Details" text box
+4: Click the button "Create Item"
+</t>
+    </r>
+  </si>
+  <si>
+    <t>The image shouldn't be larger than 320px wide or high.
+The description shouldn't be longer than 300 characters.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +149,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="56"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,15 +202,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="1" xr:uid="{D2C70E11-1281-440A-BE57-7181D9749A6B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,7 +277,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -85,7 +293,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -97,7 +305,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -114,7 +322,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -144,12 +352,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -179,6 +404,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,13 +572,163 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52383526-DB7F-4B26-A954-2E6BA9FE2F1D}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="63.75">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="63.75">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="63.75">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Assignment B test cases
</commit_message>
<xml_diff>
--- a/Documentation/Tests Documents.xlsx
+++ b/Documentation/Tests Documents.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gquispe\Documents\Stensul\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gquispe\Documents\Stensul\QA_Test\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B10528-3315-446C-9779-698B821D68F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338BB082-D6F0-476A-8053-9D3A4A5397F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DF972AE6-939A-434D-A067-644AAF37E1F0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Assignment A" sheetId="1" r:id="rId1"/>
+    <sheet name="Assignment B" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -69,29 +70,50 @@
     <t>TC5</t>
   </si>
   <si>
+    <t>Create an item</t>
+  </si>
+  <si>
+    <t>Edit another existing item</t>
+  </si>
+  <si>
+    <t>Delete the item created</t>
+  </si>
+  <si>
+    <t>Check max long in description</t>
+  </si>
+  <si>
+    <t>The new item should be displayed on the "List of Items" section.</t>
+  </si>
+  <si>
+    <t>The image must not be larger than 320px wide or high.
+The description must not be longer than 300 characters.</t>
+  </si>
+  <si>
+    <t>The new description should be displayed on the selected Item.</t>
+  </si>
+  <si>
+    <t>The "Create Item" button should be disabled.</t>
+  </si>
+  <si>
+    <t>5- Check if exist in the list the item with text “Creators: Matt Duffer, Ross Duffer”</t>
+  </si>
+  <si>
     <t xml:space="preserve">1: Navigate to http://immense-hollows-74271.herokuapp.com/
-2:  
-3: 
-4: 
+2: Search for the text "Creators: Matt Duffer, Ross Duffer" on every item's description of the "List of Items" section.
 </t>
   </si>
   <si>
-    <t>Create an item</t>
-  </si>
-  <si>
-    <t>Edit another existing item</t>
-  </si>
-  <si>
-    <t>Delete the item created</t>
-  </si>
-  <si>
-    <t>Check max long in description</t>
-  </si>
-  <si>
-    <t>5- Check if exist in the list the item with text “ Creators: Matt Duffer, Ross Duffer ”</t>
-  </si>
-  <si>
-    <t>The new item should be displayed on the "List of Items" section.</t>
+    <t>Should be able to document if the item exists or not.</t>
+  </si>
+  <si>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>Create an item with a 300 characters long description with no spaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The image must not be larger than 320px wide or high.
+</t>
   </si>
   <si>
     <r>
@@ -104,7 +126,7 @@
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
-      <t>Click the button "Choose a file" and select a jpg image</t>
+      <t>Click the button "Choose a file" and select a jpg image.</t>
     </r>
     <r>
       <rPr>
@@ -124,14 +146,112 @@
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">3: Enter the item description on the "Item Details" text box
-4: Click the button "Create Item"
+      <t xml:space="preserve">3: Enter a 300 characters long item description with no spaces on the "Item Details" text box.
+4: Click the button "Create Item".
 </t>
     </r>
   </si>
   <si>
-    <t>The image shouldn't be larger than 320px wide or high.
-The description shouldn't be longer than 300 characters.</t>
+    <t xml:space="preserve">1: Navigate to http://immense-hollows-74271.herokuapp.com/
+2: Click the "Edit" button of an item from the "List of Items" section.
+3: Enter a new item description on the "Item Details" text box.
+4: Click the button "Update Item".
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Navigate to http://immense-hollows-74271.herokuapp.com/
+2: Click the "Delete" button of the item previously created on TC1.
+3: Click the "Yes, delete it!" button.
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1: Navigate to http://immense-hollows-74271.herokuapp.com/
+2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Click the button "Choose a file" and select a jpg image.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3: Enter the item description on the "Item Details" text box.
+4: Click the button "Create Item".
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Navigate to http://immense-hollows-74271.herokuapp.com/
+2: Enter an item description of 301 characters on the "Item Details" text box.
+</t>
+  </si>
+  <si>
+    <t>The item should be removed from the "List of Items" section.</t>
+  </si>
+  <si>
+    <t>The selected item must be different from the one created on TC1.
+The new description must no be longer than 300 characters.</t>
+  </si>
+  <si>
+    <t>None.</t>
+  </si>
+  <si>
+    <t>The "Edit" button and "Delete" button of the new item should be displayed on the "List of Items" section.</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Navigate to http://immense-hollows-74271.herokuapp.com/
+2: Click the "Edit" button of an item from the "List of Items" section.
+3: Click the button "Choose a file" and select a jpg image.
+4: Click the button "Update Item".
+</t>
+  </si>
+  <si>
+    <t>Edit the image of an item</t>
+  </si>
+  <si>
+    <t>The new image should be displayed on the selected Item.</t>
+  </si>
+  <si>
+    <t>The image must not be larger than 320px wide or high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check only jpg, png or gif images are available for selection by default </t>
+  </si>
+  <si>
+    <t>1: Navigate to http://immense-hollows-74271.herokuapp.com/
+2: Click the button "Choose a file".</t>
+  </si>
+  <si>
+    <t>Shoudn't be able to select an image with a format different from "jpg", "png" or "gif".</t>
   </si>
 </sst>
 </file>
@@ -235,14 +355,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -255,8 +369,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -573,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52383526-DB7F-4B26-A954-2E6BA9FE2F1D}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -584,149 +701,267 @@
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="63.75">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="63.75">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="63.75">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="51">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="51">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="F6" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="63.75" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="63.75">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="5" t="s">
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" ht="63.75">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="63.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="63.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="6"/>
+      <c r="F7" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
+  <mergeCells count="6">
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F2"/>
-    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B91E5F6-5380-45F3-9D20-DD157DD3F4DA}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="76.5">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="63.75">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="38.25">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>